<commit_message>
Update admin/bank teller traceability matrix
</commit_message>
<xml_diff>
--- a/documents/admin_requirements_traceability_matrix.xlsx
+++ b/documents/admin_requirements_traceability_matrix.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Project Manager</t>
   </si>
@@ -84,12 +84,6 @@
     <t>Admin Log in</t>
   </si>
   <si>
-    <t>Admin must be able to log out</t>
-  </si>
-  <si>
-    <t>Admin Log out</t>
-  </si>
-  <si>
     <t>Create registration</t>
   </si>
   <si>
@@ -100,19 +94,6 @@
   </si>
   <si>
     <t>Successful</t>
-  </si>
-  <si>
-    <t>Jan 4: Testing started
-Jan 11: Error reported
-Jan 18: I can’t log in yet
-Jan 19: I can successfully log in now</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jan 4: Testing started
-Jan 11:  Error reported
-Jan 18: I still cannot create an account.
-Jan 19: I can successfully register now
-</t>
   </si>
   <si>
     <t>Jan 4: Testing started
@@ -133,30 +114,60 @@
     <t>Admin Log in with OTP</t>
   </si>
   <si>
-    <t>Jan 18: Started testing
-Jane 19: I can successfully log out now</t>
-  </si>
-  <si>
-    <t>In-progress</t>
-  </si>
-  <si>
-    <t>Jan 13: Testing started
-Jan 14: Error reported
-Jan 19: I can successfully log in, but there is no SMS for OTP yet; it is still console-based</t>
-  </si>
-  <si>
-    <t>Jan 16: Testing started
-Jan 17: Still in progress
-Jan 18: An error occurs; cannot view my transaction history.
-Jane 19: I can now view the transaction history feature successfully.</t>
-  </si>
-  <si>
     <t>Jan 4: Testing started
 Jan 18: Still in progress
 Jan 19: The withdrawal feature is now working successfully.</t>
   </si>
   <si>
     <t>HyperTechs</t>
+  </si>
+  <si>
+    <t>The account balance will be displayed, indicating whether it is sufficient or not, during deposit and withdrawal transactions.</t>
+  </si>
+  <si>
+    <t>Account balance will be displayed</t>
+  </si>
+  <si>
+    <t>Jan 24: Testing started
+Jan 25: Error reported
+Jan 26: The account balance feature is now successful</t>
+  </si>
+  <si>
+    <t>Log out</t>
+  </si>
+  <si>
+    <t>The admin must have the ability to log out, 
+with a confirmation prompt.</t>
+  </si>
+  <si>
+    <t>Jan 18: Started testing
+Jan 19: Admin can successfully log out now, but the confirmation prompt is not yet enabled.
+Jan 27: The admin can now successfully log out with a logout confirmation. This confirmation informs that logging out will terminate the current session, and users will need to reauthenticate to access their account again.</t>
+  </si>
+  <si>
+    <t>Jan 16: Testing started
+Jan 17: Still in progress
+Jan 18: An error occurs; cannot view the transaction history.
+Jane 19: Admin can now view the transaction history feature successfully.</t>
+  </si>
+  <si>
+    <t>Jan 13: Testing started
+Jan 14: Error reported
+Jan 19: Admin can successfully log in, but there is no SMS for OTP yet; it is still console-based
+Jan 26: Admin can successfully log in now with OTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 4: Testing started
+Jan 11:  Error reported
+Jan 18: Still cannot create an account.
+Jan 19: Admin can successfully register now
+</t>
+  </si>
+  <si>
+    <t>Jan 4: Testing started
+Jan 11: Error reported
+Jan 18: Admin can’t log in yet
+Jan 19: Admin can successfully log in now</t>
   </si>
 </sst>
 </file>
@@ -300,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -333,26 +344,32 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -850,10 +867,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:F14"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="88" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:F6"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,30 +885,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="23"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:6" ht="22.2" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="24" t="s">
+      <c r="A3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="26"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -900,10 +917,10 @@
       <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
@@ -912,16 +929,16 @@
       <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="28"/>
+        <v>20</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
@@ -930,148 +947,166 @@
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="32"/>
+    </row>
+    <row r="8" spans="1:6" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>3</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:6" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>4</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>5</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>6</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="32"/>
+    </row>
+    <row r="12" spans="1:6" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="30"/>
+    </row>
+    <row r="13" spans="1:6" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>8</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="C13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="30"/>
-    </row>
-    <row r="8" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
-        <v>3</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="F13" s="36"/>
+    </row>
+    <row r="14" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>9</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>4</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="28"/>
-    </row>
-    <row r="10" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <v>5</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="30"/>
-    </row>
-    <row r="11" spans="1:6" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>6</v>
-      </c>
-      <c r="B11" s="13" t="s">
+      <c r="D14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="27" t="s">
+      <c r="E14" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="28"/>
-    </row>
-    <row r="12" spans="1:6" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
-        <v>7</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="34"/>
-    </row>
-    <row r="13" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15">
-        <v>8</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="36"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
+      <c r="F14" s="38"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>